<commit_message>
Updates to rubrics and instructions
</commit_message>
<xml_diff>
--- a/LabStarters/Lab05/Lab5Rubric-CIS195.xlsx
+++ b/LabStarters/Lab05/Lab5Rubric-CIS195.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CIS195-CourseMaterials/LabStarters/Lab05/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CIS195-CourseMaterials\LabStarters\Lab05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B18AB08-C007-AB49-B8EC-5D650C6B3361}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6863906F-ACB1-4A4E-8EF9-07ADFF3AFA5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="14160" windowHeight="14740" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="36648" yWindow="-1488" windowWidth="16128" windowHeight="13200" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Rubric" sheetId="1" r:id="rId1"/>
+    <sheet name="Score" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>Requirements:</t>
   </si>
@@ -86,13 +95,19 @@
   </si>
   <si>
     <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Should be in the external CSS</t>
+  </si>
+  <si>
+    <t>Margin is fixed, but not width</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,15 +139,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,13 +160,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,23 +480,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -502,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -513,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -524,7 +529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -535,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -546,7 +551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -557,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -568,7 +573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -581,12 +586,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -597,7 +602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -608,7 +613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -619,7 +624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -630,7 +635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -641,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -652,7 +657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -663,7 +668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
@@ -674,7 +679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -687,45 +692,47 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="5">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
         <f>SUM(B9,B21)</f>
         <v>50</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="1">
         <f>SUM(C9,C21)</f>
         <v>50</v>
       </c>
+      <c r="D22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:C22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -736,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -747,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -755,10 +762,13 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -768,8 +778,11 @@
       <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -780,7 +793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -791,7 +804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -802,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -812,15 +825,15 @@
       </c>
       <c r="C9" s="3">
         <f>SUM(C3:C8)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -831,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -842,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -853,7 +866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -864,7 +877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -875,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -886,7 +899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -897,7 +910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
@@ -908,7 +921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -921,17 +934,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="5">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
         <f>SUM(B9,B21)</f>
         <v>50</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="1">
         <f>SUM(C9,C21)</f>
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>